<commit_message>
add one parapraph to summary
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B353B2F3-1FED-4D56-B198-CF6D7CFA0633}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC4E150-FA04-4C8F-A9C4-90B1D71AE58B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="1335" windowWidth="23250" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3341,10 +3341,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>